<commit_message>
Test both xls/xlsx files. Check that it can both read/write checkboxes.
</commit_message>
<xml_diff>
--- a/CheckboxLink/sample.xlsx
+++ b/CheckboxLink/sample.xlsx
@@ -47,6 +47,7 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Geneva"/>
     </font>
   </fonts>
@@ -88,7 +89,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$B$33" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$B$33" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -100,15 +101,15 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$35" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$35" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$35" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$D$35" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$36" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$36" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
@@ -915,9 +916,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B33" sqref="B33:G36"/>
     </sheetView>
   </sheetViews>
@@ -955,6 +956,24 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4">
+      <c r="C35" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4">
+      <c r="C36" s="1" t="b">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>